<commit_message>
commoy on 1th august 2025
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="402">
   <si>
     <t>TOPIC</t>
   </si>
@@ -315,9 +316,6 @@
     <t>https://leetcode.com/problems/valid-parentheses/</t>
   </si>
   <si>
-    <t>Valid Parenthesis</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/decode-string/</t>
   </si>
   <si>
@@ -610,6 +608,621 @@
   </si>
   <si>
     <t>Contains Duplicate</t>
+  </si>
+  <si>
+    <t>BACKTRACKING</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combinations/</t>
+  </si>
+  <si>
+    <t>subsets</t>
+  </si>
+  <si>
+    <t>subsets 2</t>
+  </si>
+  <si>
+    <t>combinations</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutations/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutations-ii/</t>
+  </si>
+  <si>
+    <t>Permistations (Order Matters)</t>
+  </si>
+  <si>
+    <t>Subsets / Combinations (Order doesn't matter)</t>
+  </si>
+  <si>
+    <t>permutations</t>
+  </si>
+  <si>
+    <t>permutations 2</t>
+  </si>
+  <si>
+    <t>Combination Sum (Hybrid)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum-iii/</t>
+  </si>
+  <si>
+    <t>Combination sum</t>
+  </si>
+  <si>
+    <t>combination sum 2</t>
+  </si>
+  <si>
+    <t>combination sum 3</t>
+  </si>
+  <si>
+    <t>Grid / Matrix Traversal (Pathfinding)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-search/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-with-maximum-gold/</t>
+  </si>
+  <si>
+    <t>Partitioning Problems</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-partitioning/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/restore-ip-addresses/</t>
+  </si>
+  <si>
+    <t>Constraint Satisfaction Problems</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/n-queens/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sudoku-solver/</t>
+  </si>
+  <si>
+    <t>word search</t>
+  </si>
+  <si>
+    <t>word search 2</t>
+  </si>
+  <si>
+    <t>word search 3</t>
+  </si>
+  <si>
+    <t>palindrome partitioning</t>
+  </si>
+  <si>
+    <t>restore ip address</t>
+  </si>
+  <si>
+    <t>nQueens</t>
+  </si>
+  <si>
+    <t>Sudoku</t>
+  </si>
+  <si>
+    <t>Simulation &amp; State Management</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/design-browser-history/</t>
+  </si>
+  <si>
+    <t>Simple Stack Implementation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/min-stack/</t>
+  </si>
+  <si>
+    <t>Gathering and Post-Processing Data</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-k-sorted-lists/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-all-duplicates-in-an-array/</t>
+  </si>
+  <si>
+    <t>Baseball game</t>
+  </si>
+  <si>
+    <t>crawler log folder</t>
+  </si>
+  <si>
+    <t>design browser history</t>
+  </si>
+  <si>
+    <t>simplify pat</t>
+  </si>
+  <si>
+    <t>find all duplicates in an array</t>
+  </si>
+  <si>
+    <t>ARRAYLIST</t>
+  </si>
+  <si>
+    <t>LINKEDLIST</t>
+  </si>
+  <si>
+    <t>Fast &amp; Slow Pointers (Floyd's Tortoise and Hare)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/middle-of-the-linked-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-nth-node-from-end-of-list/</t>
+  </si>
+  <si>
+    <t>Classic Pointer Manipulation (Reversal &amp; Reordering)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reorder-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/odd-even-linked-list/</t>
+  </si>
+  <si>
+    <t>The Dummy Head / Sentinel Node Trick</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-two-numbers/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/</t>
+  </si>
+  <si>
+    <t>Merging &amp; Sorting</t>
+  </si>
+  <si>
+    <t>merge k sorted arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-list/</t>
+  </si>
+  <si>
+    <t>Intersection &amp; Reference-Based Problems</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/intersection-of-two-linked-lists/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/copy-list-with-random-pointer/</t>
+  </si>
+  <si>
+    <t>DOUBLY LINKEDLIST</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lru-cache/</t>
+  </si>
+  <si>
+    <t>Implementing High-Performance Caches &amp; Queues</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lfu-cache/</t>
+  </si>
+  <si>
+    <t>Bidirectional Sequence Management</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flatten-a-multilevel-doubly-linked-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/design-linked-list/</t>
+  </si>
+  <si>
+    <t>Round-Robin &amp; Looping Logic</t>
+  </si>
+  <si>
+    <t>CIRCULAR LINKEDLIST</t>
+  </si>
+  <si>
+    <t>Find Winner of Circular Game (Josephus Problem)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-into-a-sorted-circular-linked-list/</t>
+  </si>
+  <si>
+    <t>Cycle Detection &amp; Entry Point Finding</t>
+  </si>
+  <si>
+    <t>Matching &amp; Validation (Balanced Parentheses)</t>
+  </si>
+  <si>
+    <t>STACK</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-outermost-parentheses/</t>
+  </si>
+  <si>
+    <t>Monotonic Stack (Next/Previous Greater/Smaller Element)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/next-greater-element-i/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/next-greater-element-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/daily-temperatures/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/largest-rectangle-in-histogram/</t>
+  </si>
+  <si>
+    <t>Expression Evaluation &amp; Parsing</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/basic-calculator/</t>
+  </si>
+  <si>
+    <t>Simulation &amp; Path Management</t>
+  </si>
+  <si>
+    <t>Design a Specialized Stack</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/design-a-stack-with-increment-operation/</t>
+  </si>
+  <si>
+    <t>QUEUE</t>
+  </si>
+  <si>
+    <t>BFS on a Grid/Matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotting-oranges/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/01-matrix/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-islands/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shortest-path-in-binary-matrix/</t>
+  </si>
+  <si>
+    <t>BFS on a Tree (Level Order Traversal)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-zigzag-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Sequential Processing &amp; Simulation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-recent-calls/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/dota2-senate/</t>
+  </si>
+  <si>
+    <t>Design Problems (Using Queues)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-stack-using-queues/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-queue-using-stacks/</t>
+  </si>
+  <si>
+    <t>Sliding Window Minimum/Maximum (using a Deque)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sliding-window-maximum/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> QUEUE</t>
+  </si>
+  <si>
+    <t>DEQUEUE</t>
+  </si>
+  <si>
+    <t>Monotonic Deque for Sliding Window Min/Max</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-continuous-subarray-with-absolute-diff-less-than-or-equal-to-limit/</t>
+  </si>
+  <si>
+    <t>0-1 Breadth-First Search (0-1 BFS)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-cost-to-make-at-least-one-valid-path-in-a-grid/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shortest-path-in-a-grid-with-obstacles-elimination/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-obstacle-removal-to-reach-corner/</t>
+  </si>
+  <si>
+    <t>GREEDY ALGO</t>
+  </si>
+  <si>
+    <t>Interval Scheduling &amp; Partitioning</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/meeting-rooms-ii/</t>
+  </si>
+  <si>
+    <t>Maximizing by Picking Items</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-units-on-a-truck/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/gas-station/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/assign-cookies/</t>
+  </si>
+  <si>
+    <t>Greedy Pathfinding / "Jump" Problems</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/jump-game/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/jump-game-ii/</t>
+  </si>
+  <si>
+    <t>Partitioning &amp; Slicing</t>
+  </si>
+  <si>
+    <t>Task Scheduling &amp; String Reorganization</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/task-scheduler/</t>
+  </si>
+  <si>
+    <t>BINARY TREE</t>
+  </si>
+  <si>
+    <t>The Foundation: Tree Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-preorder-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-postorder-traversal/</t>
+  </si>
+  <si>
+    <t>Validation &amp; Properties</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/validate-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/symmetric-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balanced-binary-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t>Path Sum Problems</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-iii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-maximum-path-sum/</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor (LCA)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree/</t>
+  </si>
+  <si>
+    <t>Tree Construction from Traversals</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-binary-tree-from-inorder-and-postorder-traversal/</t>
+  </si>
+  <si>
+    <t>Serialization and Deserialization</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/serialize-and-deserialize-binary-tree/</t>
+  </si>
+  <si>
+    <t>Tree Views &amp; Level-Based Problems</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-right-side-view/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subtree-of-another-tree/</t>
+  </si>
+  <si>
+    <t>BINART SEARCCH TREES</t>
+  </si>
+  <si>
+    <t>Search, Insertion, and Deletion</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-in-a-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-into-a-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/delete-node-in-a-bst/</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Finding K-th Smallest / Largest Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in a BST</t>
+  </si>
+  <si>
+    <t>Kth Smallest Element in a BST</t>
+  </si>
+  <si>
+    <t>Finding Specific Relationship Nodes (LCA, Successor)</t>
+  </si>
+  <si>
+    <t>Inorder Successor in BST</t>
+  </si>
+  <si>
+    <t>Construction, Conversion, and "Fixing"</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/convert-sorted-array-to-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balance-a-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/recover-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/convert-bst-to-greater-tree/</t>
+  </si>
+  <si>
+    <t>Top K Elements (Largest, Smallest, Frequent)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-largest-element-in-an-array/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/top-k-frequent-elements/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-closest-points-to-origin/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-k-pairs-with-smallest-sums/</t>
+  </si>
+  <si>
+    <t>Merging K Sorted Data Structures</t>
+  </si>
+  <si>
+    <t>Finding the Median (Two Heaps Pattern)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-median-from-data-stream/</t>
+  </si>
+  <si>
+    <t>Greedy / Scheduling Problems</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ipo/</t>
+  </si>
+  <si>
+    <t>PRIORTIY QUEUES/HEAPS</t>
+  </si>
+  <si>
+    <t>HASHING</t>
+  </si>
+  <si>
+    <t>Frequency Counting &amp; Existence Checks</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ransom-note/</t>
+  </si>
+  <si>
+    <t>The "Two-Sum" Pattern &amp; Its Variations</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/4sum-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/contiguous-array/</t>
+  </si>
+  <si>
+    <t>Grouping and Categorization</t>
+  </si>
+  <si>
+    <t>Subarray / Substring Problems (Combined with Prefix Sums)</t>
+  </si>
+  <si>
+    <t>middle of the linked list</t>
+  </si>
+  <si>
+    <t>remove from end of linkedlist</t>
+  </si>
+  <si>
+    <t>LinkedList Cycle 2</t>
+  </si>
+  <si>
+    <t>LinkedList Cycle 1</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>DONE;</t>
+  </si>
+  <si>
+    <t>reverse _Linked_list 2</t>
   </si>
 </sst>
 </file>
@@ -678,7 +1291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -718,6 +1331,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1020,20 +1636,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:F332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H151" sqref="H151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.81640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="20.90625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="53.08984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="44.08984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="69.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="92" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
@@ -1586,28 +2202,22 @@
       <c r="A56" s="5">
         <v>39</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>40</v>
       </c>
+      <c r="B57" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="D57" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
@@ -1615,10 +2225,10 @@
         <v>41</v>
       </c>
       <c r="D58" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -1629,13 +2239,13 @@
         <v>86</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -1643,10 +2253,10 @@
         <v>43</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -1654,10 +2264,10 @@
         <v>44</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -1668,13 +2278,13 @@
         <v>86</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="E64" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -1682,10 +2292,10 @@
         <v>46</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -1693,10 +2303,10 @@
         <v>47</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -1704,10 +2314,10 @@
         <v>48</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -1715,10 +2325,10 @@
         <v>49</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -1729,13 +2339,13 @@
         <v>86</v>
       </c>
       <c r="C70" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="E70" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -1743,10 +2353,10 @@
         <v>51</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -1754,16 +2364,16 @@
         <v>52</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -1771,10 +2381,10 @@
         <v>53</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -1782,10 +2392,10 @@
         <v>54</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -1793,10 +2403,10 @@
         <v>55</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -1804,16 +2414,16 @@
         <v>56</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C80" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
@@ -1821,10 +2431,10 @@
         <v>57</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
@@ -1832,10 +2442,10 @@
         <v>58</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -1843,10 +2453,10 @@
         <v>59</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
@@ -1854,16 +2464,16 @@
         <v>60</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C85" t="s">
+        <v>163</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
@@ -1871,10 +2481,10 @@
         <v>61</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
@@ -1882,10 +2492,10 @@
         <v>62</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -1893,16 +2503,16 @@
         <v>63</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C89" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
@@ -1910,10 +2520,10 @@
         <v>64</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
@@ -1921,16 +2531,16 @@
         <v>65</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C92" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E92" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
@@ -1938,10 +2548,10 @@
         <v>66</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
@@ -1949,10 +2559,10 @@
         <v>67</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
@@ -1960,16 +2570,16 @@
         <v>68</v>
       </c>
       <c r="B98" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="D98" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
@@ -1977,10 +2587,10 @@
         <v>69</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
@@ -1988,10 +2598,10 @@
         <v>70</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
@@ -1999,10 +2609,10 @@
         <v>71</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
@@ -2010,10 +2620,10 @@
         <v>72</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
@@ -2021,16 +2631,16 @@
         <v>73</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C104" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
@@ -2038,10 +2648,10 @@
         <v>74</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
@@ -2049,10 +2659,10 @@
         <v>75</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
@@ -2060,10 +2670,10 @@
         <v>76</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
@@ -2071,16 +2681,16 @@
         <v>77</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C109" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
@@ -2088,10 +2698,10 @@
         <v>78</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
@@ -2099,16 +2709,16 @@
         <v>79</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C112" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E112" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
@@ -2116,10 +2726,10 @@
         <v>80</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
@@ -2127,10 +2737,10 @@
         <v>81</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
@@ -2138,10 +2748,1561 @@
         <v>82</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="5">
+        <v>83</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="5">
+        <v>84</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="5">
+        <v>85</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" s="5">
+        <v>86</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" s="5">
+        <v>87</v>
+      </c>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" s="5">
+        <v>88</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" s="5">
+        <v>89</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" s="5">
+        <v>90</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" s="5">
+        <v>91</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" s="5">
+        <v>92</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" s="5">
+        <v>93</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" s="5">
+        <v>94</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" s="5">
+        <v>95</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" s="5">
+        <v>96</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" s="5">
+        <v>97</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140" s="5">
+        <v>98</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141" s="5">
+        <v>99</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142" s="5">
+        <v>100</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C143" s="2"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" s="5">
+        <v>101</v>
+      </c>
+      <c r="B144" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146" s="5">
+        <v>102</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C146" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147" s="5">
+        <v>103</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A151" s="5">
+        <v>104</v>
+      </c>
+      <c r="B151" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C151" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E151" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A152" s="5">
+        <v>105</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A153" s="5">
+        <v>106</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A154" s="5">
+        <v>107</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E154" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A156" s="5">
+        <v>108</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C156" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E156" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A157" s="5">
+        <v>109</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A158" s="5">
+        <v>110</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A159" s="5">
+        <v>111</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" s="5">
+        <v>112</v>
+      </c>
+      <c r="B161" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" s="5">
+        <v>113</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163" s="5">
+        <v>114</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165" s="5">
+        <v>115</v>
+      </c>
+      <c r="B165" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" s="5">
+        <v>116</v>
+      </c>
+      <c r="C166" s="2"/>
+      <c r="E166" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167" s="5">
+        <v>117</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" s="5">
+        <v>118</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170" s="5">
+        <v>119</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174" s="5">
+        <v>120</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C174" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175" s="5">
+        <v>121</v>
+      </c>
+      <c r="E175" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A177" s="5">
+        <v>122</v>
+      </c>
+      <c r="B177" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D177" s="2"/>
+      <c r="E177" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178" s="5">
+        <v>123</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182" s="5">
+        <v>124</v>
+      </c>
+      <c r="B182" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183" s="5">
+        <v>125</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A185" s="5">
+        <v>126</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A186" s="5">
+        <v>127</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A190" s="5">
+        <v>128</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A191" s="5">
+        <v>129</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A193" s="5">
+        <v>130</v>
+      </c>
+      <c r="B193" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C193" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A194" s="5">
+        <v>131</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A195" s="5">
+        <v>132</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A196" s="5">
+        <v>133</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A198" s="5">
+        <v>134</v>
+      </c>
+      <c r="B198" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" s="5">
+        <v>135</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201" s="5">
+        <v>136</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A202" s="5">
+        <v>137</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A204" s="5">
+        <v>138</v>
+      </c>
+      <c r="B204" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A205" s="5">
+        <v>139</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A209" s="5">
+        <v>140</v>
+      </c>
+      <c r="B209" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A210" s="5">
+        <v>141</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211" s="5">
+        <v>142</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212" s="5">
+        <v>143</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214" s="5">
+        <v>144</v>
+      </c>
+      <c r="B214" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215" s="5">
+        <v>145</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216" s="5">
+        <v>146</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218" s="5">
+        <v>147</v>
+      </c>
+      <c r="B218" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A219" s="5">
+        <v>148</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A220" s="5">
+        <v>149</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A222" s="5">
+        <v>150</v>
+      </c>
+      <c r="B222" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A223" s="5">
+        <v>151</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A225" s="5">
+        <v>152</v>
+      </c>
+      <c r="B225" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A229" s="5">
+        <v>153</v>
+      </c>
+      <c r="B229" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A230" s="5">
+        <v>154</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A232" s="5">
+        <v>155</v>
+      </c>
+      <c r="B232" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A233" s="5">
+        <v>156</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A234" s="5">
+        <v>157</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A238" s="5">
+        <v>158</v>
+      </c>
+      <c r="B238" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A239" s="5">
+        <v>159</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A240" s="5">
+        <v>160</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A241" s="5">
+        <v>161</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A243" s="5">
+        <v>162</v>
+      </c>
+      <c r="B243" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A244" s="5">
+        <v>163</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A245" s="5">
+        <v>164</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A247" s="5">
+        <v>165</v>
+      </c>
+      <c r="B247" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A248" s="5">
+        <v>166</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A250" s="5">
+        <v>167</v>
+      </c>
+      <c r="B250" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A252" s="5">
+        <v>168</v>
+      </c>
+      <c r="B252" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E252" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A253" s="5">
+        <v>169</v>
+      </c>
+      <c r="E253" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A257" s="5">
+        <v>170</v>
+      </c>
+      <c r="B257" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C257" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="E257" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A258" s="5">
+        <v>171</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A259" s="5">
+        <v>172</v>
+      </c>
+      <c r="E259" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A260" s="5">
+        <v>173</v>
+      </c>
+      <c r="E260" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C261" s="2"/>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A262" s="5">
+        <v>174</v>
+      </c>
+      <c r="B262" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E262" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A263" s="5">
+        <v>175</v>
+      </c>
+      <c r="E263" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A264" s="5">
+        <v>176</v>
+      </c>
+      <c r="E264" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A266" s="5">
+        <v>177</v>
+      </c>
+      <c r="B266" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E266" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A267" s="5">
+        <v>178</v>
+      </c>
+      <c r="E267" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A268" s="5">
+        <v>179</v>
+      </c>
+      <c r="E268" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A269" s="5">
+        <v>180</v>
+      </c>
+      <c r="E269" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A271" s="5">
+        <v>181</v>
+      </c>
+      <c r="B271" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E271" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A272" s="5">
+        <v>182</v>
+      </c>
+      <c r="E272" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A274" s="5">
+        <v>183</v>
+      </c>
+      <c r="B274" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C274" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="E274" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A275" s="5">
+        <v>184</v>
+      </c>
+      <c r="E275" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A277" s="5">
+        <v>185</v>
+      </c>
+      <c r="B277" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E277" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A279" s="5">
+        <v>186</v>
+      </c>
+      <c r="B279" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E279" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A280" s="5">
+        <v>187</v>
+      </c>
+      <c r="E280" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A281" s="5">
+        <v>188</v>
+      </c>
+      <c r="E281" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A285" s="5">
+        <v>189</v>
+      </c>
+      <c r="B285" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E285" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A286" s="5">
+        <v>190</v>
+      </c>
+      <c r="E286" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A287" s="5">
+        <v>191</v>
+      </c>
+      <c r="E287" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A289" s="5">
+        <v>192</v>
+      </c>
+      <c r="B289" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E290"/>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A291" s="5">
+        <v>193</v>
+      </c>
+      <c r="B291" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E291" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A292" s="5">
+        <v>194</v>
+      </c>
+      <c r="D292" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A294" s="5">
+        <v>195</v>
+      </c>
+      <c r="B294" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E294" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A295" s="5">
+        <v>196</v>
+      </c>
+      <c r="D295" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A297" s="5">
+        <v>197</v>
+      </c>
+      <c r="B297" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E297" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A298" s="5">
+        <v>198</v>
+      </c>
+      <c r="E298" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A299" s="5">
+        <v>199</v>
+      </c>
+      <c r="E299" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A300" s="5">
+        <v>200</v>
+      </c>
+      <c r="E300" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A304" s="5">
+        <v>201</v>
+      </c>
+      <c r="B304" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E304" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A305" s="5">
+        <v>202</v>
+      </c>
+      <c r="E305" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A306" s="5">
+        <v>203</v>
+      </c>
+      <c r="E306" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A307" s="5">
+        <v>204</v>
+      </c>
+      <c r="E307" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A309" s="5">
+        <v>205</v>
+      </c>
+      <c r="B309" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E309" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A311" s="5">
+        <v>206</v>
+      </c>
+      <c r="B311" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E311" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A313" s="5">
+        <v>207</v>
+      </c>
+      <c r="B313" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E313" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A314" s="5">
+        <v>208</v>
+      </c>
+      <c r="E314" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A315" s="5">
+        <v>209</v>
+      </c>
+      <c r="E315" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A319" s="5">
+        <v>210</v>
+      </c>
+      <c r="B319" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="C319" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="E319" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A320" s="5">
+        <v>211</v>
+      </c>
+      <c r="E320" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A321" s="5">
+        <v>212</v>
+      </c>
+      <c r="E321" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A322" s="5">
+        <v>213</v>
+      </c>
+      <c r="E322" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A324" s="5">
+        <v>214</v>
+      </c>
+      <c r="B324" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E324" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A325" s="5">
+        <v>215</v>
+      </c>
+      <c r="E325" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A326" s="5">
+        <v>216</v>
+      </c>
+      <c r="E326" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A328" s="5">
+        <v>217</v>
+      </c>
+      <c r="B328" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E328" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A329" s="5">
+        <v>218</v>
+      </c>
+      <c r="E329" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A331" s="5">
+        <v>219</v>
+      </c>
+      <c r="B331" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E331" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A332" s="5">
+        <v>220</v>
+      </c>
+      <c r="E332" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2159,9 +4320,16 @@
     <hyperlink ref="E23" r:id="rId11"/>
     <hyperlink ref="E24" r:id="rId12"/>
     <hyperlink ref="E61" r:id="rId13"/>
+    <hyperlink ref="E117" r:id="rId14"/>
+    <hyperlink ref="E152" r:id="rId15"/>
+    <hyperlink ref="E154" r:id="rId16"/>
+    <hyperlink ref="E151" r:id="rId17"/>
+    <hyperlink ref="E153" r:id="rId18"/>
+    <hyperlink ref="E156" r:id="rId19"/>
+    <hyperlink ref="E157" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
dated 21st au 2025
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="401">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1217,9 +1216,6 @@
   </si>
   <si>
     <t>Reverse Linked List</t>
-  </si>
-  <si>
-    <t>DONE;</t>
   </si>
   <si>
     <t>reverse _Linked_list 2</t>
@@ -1638,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2670,7 +2666,7 @@
       <c r="D106" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E106" s="9" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2681,7 +2677,7 @@
       <c r="D107" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E107" s="9" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2736,40 +2732,40 @@
         <v>190</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>80</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E113" s="9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>81</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E114" s="3" t="s">
+      <c r="E114" s="9" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>82</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="E115" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>83</v>
       </c>
@@ -2785,8 +2781,11 @@
       <c r="E117" s="9" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F117" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>84</v>
       </c>
@@ -2797,7 +2796,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>85</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>86</v>
       </c>
@@ -2825,7 +2824,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>87</v>
       </c>
@@ -2837,7 +2836,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>88</v>
       </c>
@@ -2854,7 +2853,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>89</v>
       </c>
@@ -2865,7 +2864,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>90</v>
       </c>
@@ -2876,7 +2875,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>91</v>
       </c>
@@ -2893,7 +2892,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>92</v>
       </c>
@@ -2904,7 +2903,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>93</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="5">
         <v>94</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>95</v>
       </c>
@@ -2943,7 +2942,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="5">
         <v>96</v>
       </c>
@@ -2956,11 +2955,14 @@
       <c r="D135" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E135" s="3" t="s">
+      <c r="E135" s="9" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F135" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="5">
         <v>97</v>
       </c>
@@ -2971,7 +2973,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" s="5">
         <v>98</v>
       </c>
@@ -2987,8 +2989,11 @@
       <c r="E140" s="9" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F140" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" s="5">
         <v>99</v>
       </c>
@@ -2999,7 +3004,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="5">
         <v>100</v>
       </c>
@@ -3010,10 +3015,10 @@
         <v>233</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C143" s="2"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" s="5">
         <v>101</v>
       </c>
@@ -3043,7 +3048,7 @@
       <c r="D146" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="E146" s="3" t="s">
+      <c r="E146" s="9" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3054,7 +3059,7 @@
       <c r="D147" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E147" s="3" t="s">
+      <c r="E147" s="9" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3137,7 +3142,7 @@
         <v>253</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>400</v>
+        <v>78</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
@@ -3145,21 +3150,24 @@
         <v>109</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E157" s="9" t="s">
         <v>254</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>400</v>
+        <v>78</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>110</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E158" s="9" t="s">
         <v>255</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
@@ -4374,9 +4382,18 @@
     <hyperlink ref="E105" r:id="rId38"/>
     <hyperlink ref="E110" r:id="rId39"/>
     <hyperlink ref="E109" r:id="rId40"/>
+    <hyperlink ref="E106" r:id="rId41"/>
+    <hyperlink ref="E107" r:id="rId42"/>
+    <hyperlink ref="E114" r:id="rId43"/>
+    <hyperlink ref="E115" r:id="rId44"/>
+    <hyperlink ref="E113" r:id="rId45"/>
+    <hyperlink ref="E147" r:id="rId46"/>
+    <hyperlink ref="E146" r:id="rId47"/>
+    <hyperlink ref="E158" r:id="rId48"/>
+    <hyperlink ref="E135" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
commit on 23rd august
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="401">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="D185" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2410,8 +2410,11 @@
       <c r="D78" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" s="9" t="s">
         <v>133</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -3040,8 +3043,11 @@
       <c r="D144" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="E144" s="3" t="s">
+      <c r="E144" s="9" t="s">
         <v>102</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
@@ -3386,6 +3392,9 @@
       <c r="E191" s="9" t="s">
         <v>281</v>
       </c>
+      <c r="F191" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" s="5">
@@ -3462,6 +3471,9 @@
       </c>
       <c r="E201" s="9" t="s">
         <v>102</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.35">
@@ -4404,9 +4416,11 @@
     <hyperlink ref="E75" r:id="rId51"/>
     <hyperlink ref="E76" r:id="rId52"/>
     <hyperlink ref="E77" r:id="rId53"/>
+    <hyperlink ref="E78" r:id="rId54"/>
+    <hyperlink ref="E144" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
 

</xml_diff>